<commit_message>
Week 5 task A
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunellauni/Documents/UWE/MachineLearning/MLPA_Tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BEEFB2D-7C88-1041-AD35-8348EFDA0D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55CE87C-6759-1D40-8948-2010E3598E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23760" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -52,6 +52,12 @@
   <si>
     <t>Linear Regression</t>
   </si>
+  <si>
+    <t>Sunella Fernando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLPA Sept21 TB2 </t>
+  </si>
 </sst>
 </file>
 
@@ -76,7 +82,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,6 +105,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -348,7 +366,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -406,9 +424,6 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -419,6 +434,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -551,7 +575,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -1870,7 +1894,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1885,7 +1909,9 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
@@ -1894,7 +1920,9 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
@@ -1969,7 +1997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2006,61 +2036,61 @@
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
@@ -2068,7 +2098,7 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="23"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13"/>

</xml_diff>